<commit_message>
Merge test into minimax
</commit_message>
<xml_diff>
--- a/Agile/Burndown.xlsx
+++ b/Agile/Burndown.xlsx
@@ -1,34 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy Fulton\315-P3-Group17\Agile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy Fulton\315-P3-Group17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF00892-7DB5-4FF3-8C06-5EE423A20CF1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A0B3B4BA-8A2D-4B2B-942E-85237B859BAF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Burndown" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -234,6 +227,12 @@
     <t>19, 21, 22, 25</t>
   </si>
   <si>
+    <t>17, 24, 27</t>
+  </si>
+  <si>
+    <t>18, 20, 28</t>
+  </si>
+  <si>
     <t>23, 26, 29, 30</t>
   </si>
   <si>
@@ -241,18 +240,12 @@
   </si>
   <si>
     <t>33, 35</t>
-  </si>
-  <si>
-    <t>18, 20, 28, 17, 24, 27</t>
-  </si>
-  <si>
-    <t>27, 20, 17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -912,10 +905,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$2:$A$14</c:f>
+              <c:f>Burndown!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>43388</c:v>
                 </c:pt>
@@ -935,24 +928,27 @@
                   <c:v>43396</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>43401</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>43402</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43403</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43404</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43405</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43407</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43408</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43409</c:v>
                 </c:pt>
               </c:numCache>
@@ -960,10 +956,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$J$2:$J$14</c:f>
+              <c:f>Burndown!$J$2:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>36</c:v>
                 </c:pt>
@@ -983,24 +979,27 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1042,10 +1041,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$2:$A$14</c:f>
+              <c:f>Burndown!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>43388</c:v>
                 </c:pt>
@@ -1065,24 +1064,27 @@
                   <c:v>43396</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>43401</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>43402</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43403</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43404</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43405</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43407</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43408</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43409</c:v>
                 </c:pt>
               </c:numCache>
@@ -1090,10 +1092,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$K$2:$K$14</c:f>
+              <c:f>Burndown!$K$2:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>36</c:v>
                 </c:pt>
@@ -1113,25 +1115,28 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19</c:v>
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1978,13 +1983,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1127760</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2309,10 +2314,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -2883,11 +2888,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2960,11 +2965,11 @@
         <v>2</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:K7" si="0">$D$17-G2</f>
+        <f>$D$18-G2</f>
         <v>36</v>
       </c>
       <c r="K2">
-        <f t="shared" si="0"/>
+        <f>$D$18-H2</f>
         <v>36</v>
       </c>
     </row>
@@ -2996,11 +3001,11 @@
         <v>3</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
+        <f>$D$18-G3</f>
         <v>35</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
+        <f>$D$18-H3</f>
         <v>35</v>
       </c>
     </row>
@@ -3024,19 +3029,19 @@
         <v>53</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G7" si="1">LEN(E4)-LEN(SUBSTITUTE(E4,",",""))+1 + G3</f>
+        <f t="shared" ref="G4:G7" si="0">LEN(E4)-LEN(SUBSTITUTE(E4,",",""))+1 + G3</f>
         <v>5</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H14" si="2">IF(ISBLANK(F4), 0, (LEN(F4)-LEN(SUBSTITUTE(F4,",",""))+1)) + H3</f>
+        <f t="shared" ref="H4:H15" si="1">IF(ISBLANK(F4), 0, (LEN(F4)-LEN(SUBSTITUTE(F4,",",""))+1)) + H3</f>
         <v>5</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f>$D$18-G4</f>
         <v>33</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f>$D$18-H4</f>
         <v>33</v>
       </c>
     </row>
@@ -3060,19 +3065,19 @@
         <v>6</v>
       </c>
       <c r="G5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f>$D$18-G5</f>
         <v>30</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
+        <f>$D$18-H5</f>
         <v>32</v>
       </c>
     </row>
@@ -3096,19 +3101,19 @@
         <v>61</v>
       </c>
       <c r="G6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f>$D$18-G6</f>
         <v>26</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
+        <f>$D$18-H6</f>
         <v>28</v>
       </c>
     </row>
@@ -3132,64 +3137,61 @@
         <v>63</v>
       </c>
       <c r="G7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f>$D$18-G7</f>
         <v>22</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
+        <f>$D$18-H7</f>
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>43402</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.17361111111111113</v>
+      <c r="A8" s="1">
+        <v>43401</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G14" si="3">LEN(E8)-LEN(SUBSTITUTE(E8,",",""))+1 + G7</f>
+        <f t="shared" ref="G8:G15" si="2">LEN(E8)-LEN(SUBSTITUTE(E8,",",""))+1 + G7</f>
+        <v>19</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J15" si="3">$D$18-G8</f>
+        <v>19</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8:K15" si="4">$D$18-H8</f>
         <v>22</v>
       </c>
-      <c r="H8">
-        <f t="shared" ref="H8:H14" si="4">IF(ISBLANK(F8), 0, (LEN(F8)-LEN(SUBSTITUTE(F8,",",""))+1)) + H7</f>
-        <v>19</v>
-      </c>
-      <c r="J8">
-        <f t="shared" ref="J8:J14" si="5">$D$17-G8</f>
-        <v>16</v>
-      </c>
-      <c r="K8">
-        <f t="shared" ref="K8:K14" si="6">$D$17-H8</f>
-        <v>19</v>
-      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>43403</v>
+      <c r="A9" s="6">
+        <v>43402</v>
       </c>
       <c r="B9" s="2">
-        <v>0.52430555555555558</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -3198,64 +3200,64 @@
         <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G9">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="3"/>
-        <v>26</v>
-      </c>
-      <c r="H9">
+        <v>16</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>43403</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="6"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>43404</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.17361111111111113</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G10">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="H10">
+        <v>12</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>43405</v>
+      <c r="A11" s="5">
+        <v>43404</v>
       </c>
       <c r="B11" s="2">
-        <v>0.52430555555555558</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -3264,31 +3266,31 @@
         <v>7</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G11">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>43407</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>52</v>
+      <c r="A12" s="1">
+        <v>43405</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.52430555555555558</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -3297,64 +3299,64 @@
         <v>7</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G12">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>43408</v>
+      <c r="A13" s="5">
+        <v>43407</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="4">
-        <v>37</v>
+      <c r="E13" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="G13">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>43409</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.17361111111111113</v>
+      <c r="A14" s="1">
+        <v>43408</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -3363,30 +3365,63 @@
         <v>7</v>
       </c>
       <c r="E14" s="4">
+        <v>37</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>43409</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.17361111111111113</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="4">
         <v>38</v>
       </c>
-      <c r="G14">
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J15">
         <f t="shared" si="3"/>
-        <v>38</v>
-      </c>
-      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="6"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>38</v>
       </c>
     </row>

</xml_diff>